<commit_message>
Commit against the changes
</commit_message>
<xml_diff>
--- a/sst.xlsx
+++ b/sst.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Main" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Tracking" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tracking" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -582,7 +582,7 @@
       </c>
       <c r="B2" s="8" t="inlineStr">
         <is>
-          <t>46926.20000000</t>
+          <t>47339.88000000</t>
         </is>
       </c>
       <c r="C2" s="8" t="inlineStr">
@@ -610,7 +610,7 @@
       </c>
       <c r="H2" s="8" t="inlineStr">
         <is>
-          <t>45900.00000000</t>
+          <t>45678.00000000</t>
         </is>
       </c>
       <c r="I2" s="8" t="n"/>
@@ -623,7 +623,7 @@
       </c>
       <c r="B3" s="8" t="inlineStr">
         <is>
-          <t>3713.21000000</t>
+          <t>3749.65000000</t>
         </is>
       </c>
       <c r="C3" s="8" t="inlineStr">
@@ -643,15 +643,15 @@
       </c>
       <c r="F3" s="8" t="inlineStr">
         <is>
-          <t>4173.63000000</t>
+          <t>4150.00000000</t>
         </is>
       </c>
       <c r="G3" s="12" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>3585.00000000</t>
+          <t>3622.29000000</t>
         </is>
       </c>
       <c r="I3" s="8" t="inlineStr">
@@ -668,7 +668,7 @@
       </c>
       <c r="B4" s="8" t="inlineStr">
         <is>
-          <t>511.00000000</t>
+          <t>523.70000000</t>
         </is>
       </c>
       <c r="C4" s="8" t="inlineStr">
@@ -688,15 +688,15 @@
       </c>
       <c r="F4" s="8" t="inlineStr">
         <is>
-          <t>574.80000000</t>
+          <t>572.00000000</t>
         </is>
       </c>
       <c r="G4" s="12" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H4" s="8" t="inlineStr">
         <is>
-          <t>507.00000000</t>
+          <t>506.00000000</t>
         </is>
       </c>
       <c r="I4" s="8" t="n"/>
@@ -709,7 +709,7 @@
       </c>
       <c r="B5" s="8" t="inlineStr">
         <is>
-          <t>5.90330000</t>
+          <t>5.89270000</t>
         </is>
       </c>
       <c r="C5" s="8" t="inlineStr">
@@ -733,11 +733,11 @@
         </is>
       </c>
       <c r="G5" s="8" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" s="8" t="inlineStr">
         <is>
-          <t>5.56640000</t>
+          <t>5.73600000</t>
         </is>
       </c>
       <c r="I5" s="8" t="n"/>
@@ -750,7 +750,7 @@
       </c>
       <c r="B6" s="8" t="inlineStr">
         <is>
-          <t>85.47000000</t>
+          <t>91.55000000</t>
         </is>
       </c>
       <c r="C6" s="8" t="inlineStr">
@@ -774,11 +774,11 @@
         </is>
       </c>
       <c r="G6" s="12" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>81.11000000</t>
+          <t>84.14000000</t>
         </is>
       </c>
       <c r="I6" s="8" t="n"/>
@@ -791,7 +791,7 @@
       </c>
       <c r="B7" s="8" t="inlineStr">
         <is>
-          <t>26.56000000</t>
+          <t>28.23000000</t>
         </is>
       </c>
       <c r="C7" s="8" t="inlineStr">
@@ -815,11 +815,11 @@
         </is>
       </c>
       <c r="G7" s="8" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>26.17000000</t>
+          <t>26.24000000</t>
         </is>
       </c>
       <c r="I7" s="8" t="n"/>
@@ -832,7 +832,7 @@
       </c>
       <c r="B8" s="8" t="inlineStr">
         <is>
-          <t>140.10000000</t>
+          <t>187.20000000</t>
         </is>
       </c>
       <c r="C8" s="8" t="inlineStr">
@@ -852,15 +852,15 @@
       </c>
       <c r="F8" s="8" t="inlineStr">
         <is>
-          <t>97.70000000</t>
+          <t>96.80000000</t>
         </is>
       </c>
       <c r="G8" s="12" t="n">
-        <v>-30</v>
+        <v>-48</v>
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>138.40000000</t>
+          <t>132.60000000</t>
         </is>
       </c>
       <c r="I8" s="8" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="B9" s="8" t="inlineStr">
         <is>
-          <t>2.09560000</t>
+          <t>2.57850000</t>
         </is>
       </c>
       <c r="C9" s="8" t="inlineStr">
@@ -897,15 +897,15 @@
       </c>
       <c r="F9" s="8" t="inlineStr">
         <is>
-          <t>2.44880000</t>
-        </is>
-      </c>
-      <c r="G9" s="11" t="n">
-        <v>16</v>
+          <t>2.59830000</t>
+        </is>
+      </c>
+      <c r="G9" s="12" t="n">
+        <v>0</v>
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
-          <t>2.03500000</t>
+          <t>2.08050000</t>
         </is>
       </c>
       <c r="I9" s="8" t="n"/>
@@ -918,7 +918,7 @@
       </c>
       <c r="B10" s="8" t="inlineStr">
         <is>
-          <t>2.52500000</t>
+          <t>2.53000000</t>
         </is>
       </c>
       <c r="C10" s="8" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="H10" s="8" t="inlineStr">
         <is>
-          <t>2.40600000</t>
+          <t>2.44000000</t>
         </is>
       </c>
       <c r="I10" s="8" t="n"/>
@@ -959,7 +959,7 @@
       </c>
       <c r="B11" s="8" t="inlineStr">
         <is>
-          <t>0.00003390</t>
+          <t>0.00003399</t>
         </is>
       </c>
       <c r="C11" s="8" t="inlineStr">
@@ -987,7 +987,7 @@
       </c>
       <c r="H11" s="8" t="inlineStr">
         <is>
-          <t>0.00003291</t>
+          <t>0.00003262</t>
         </is>
       </c>
       <c r="I11" s="8" t="n"/>
@@ -1000,17 +1000,17 @@
       </c>
       <c r="B12" s="8" t="inlineStr">
         <is>
-          <t>171.02000000</t>
+          <t>178.35000000</t>
         </is>
       </c>
       <c r="C12" s="8" t="inlineStr">
         <is>
-          <t>148.04000000</t>
+          <t>149.60000000</t>
         </is>
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>13-12-21</t>
+          <t>14-12-21</t>
         </is>
       </c>
       <c r="E12" s="8" t="inlineStr">
@@ -1023,12 +1023,12 @@
           <t>204.75000000</t>
         </is>
       </c>
-      <c r="G12" s="8" t="n">
-        <v>19</v>
+      <c r="G12" s="12" t="n">
+        <v>14</v>
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>168.17000000</t>
+          <t>167.67000000</t>
         </is>
       </c>
       <c r="I12" s="8" t="n"/>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B13" s="8" t="inlineStr">
         <is>
-          <t>1.34000000</t>
+          <t>1.35500000</t>
         </is>
       </c>
       <c r="C13" s="8" t="inlineStr">
@@ -1065,11 +1065,11 @@
         </is>
       </c>
       <c r="G13" s="8" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>1.29700000</t>
+          <t>1.28100000</t>
         </is>
       </c>
       <c r="I13" s="8" t="n"/>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="B14" s="8" t="inlineStr">
         <is>
-          <t>100.77000000</t>
+          <t>115.54000000</t>
         </is>
       </c>
       <c r="C14" s="8" t="inlineStr">
@@ -1102,11 +1102,11 @@
       </c>
       <c r="F14" s="8" t="inlineStr">
         <is>
-          <t>89.92000000</t>
+          <t>87.46000000</t>
         </is>
       </c>
       <c r="G14" s="12" t="n">
-        <v>-10</v>
+        <v>-24</v>
       </c>
       <c r="H14" s="8" t="inlineStr">
         <is>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B15" s="8" t="inlineStr">
         <is>
-          <t>0.46619000</t>
+          <t>0.45744000</t>
         </is>
       </c>
       <c r="C15" s="8" t="inlineStr">
@@ -1147,15 +1147,15 @@
       </c>
       <c r="F15" s="8" t="inlineStr">
         <is>
-          <t>0.63075000</t>
+          <t>0.55359000</t>
         </is>
       </c>
       <c r="G15" s="8" t="n">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>0.44044000</t>
+          <t>0.44410000</t>
         </is>
       </c>
       <c r="I15" s="8" t="n"/>
@@ -1168,17 +1168,17 @@
       </c>
       <c r="B16" s="8" t="inlineStr">
         <is>
-          <t>0.83150000</t>
+          <t>0.84290000</t>
         </is>
       </c>
       <c r="C16" s="8" t="inlineStr">
         <is>
-          <t>0.76010000</t>
+          <t>0.77170000</t>
         </is>
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>13-12-21</t>
+          <t>14-12-21</t>
         </is>
       </c>
       <c r="E16" s="8" t="inlineStr">
@@ -1192,11 +1192,11 @@
         </is>
       </c>
       <c r="G16" s="8" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H16" s="8" t="inlineStr">
         <is>
-          <t>0.80200000</t>
+          <t>0.80250000</t>
         </is>
       </c>
       <c r="I16" s="8" t="n"/>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="B17" s="8" t="inlineStr">
         <is>
-          <t>10.02100000</t>
+          <t>9.02000000</t>
         </is>
       </c>
       <c r="C17" s="8" t="inlineStr">
@@ -1233,11 +1233,11 @@
         </is>
       </c>
       <c r="G17" s="12" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>8.70200000</t>
+          <t>8.91300000</t>
         </is>
       </c>
       <c r="I17" s="8" t="n"/>
@@ -1250,17 +1250,17 @@
       </c>
       <c r="B18" s="8" t="inlineStr">
         <is>
-          <t>15.48600000</t>
+          <t>15.05700000</t>
         </is>
       </c>
       <c r="C18" s="8" t="inlineStr">
         <is>
-          <t>10.51600000</t>
+          <t>10.69500000</t>
         </is>
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>12-12-21</t>
+          <t>23-12-21</t>
         </is>
       </c>
       <c r="E18" s="8" t="inlineStr">
@@ -1274,11 +1274,11 @@
         </is>
       </c>
       <c r="G18" s="12" t="n">
-        <v>-37</v>
+        <v>-35</v>
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>13.13500000</t>
+          <t>14.14600000</t>
         </is>
       </c>
       <c r="I18" s="8" t="n"/>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B19" s="8" t="inlineStr">
         <is>
-          <t>35.35000000</t>
+          <t>35.63000000</t>
         </is>
       </c>
       <c r="C19" s="8" t="inlineStr">
@@ -1314,12 +1314,12 @@
           <t>41.27000000</t>
         </is>
       </c>
-      <c r="G19" s="8" t="n">
-        <v>16</v>
+      <c r="G19" s="12" t="n">
+        <v>15</v>
       </c>
       <c r="H19" s="8" t="inlineStr">
         <is>
-          <t>33.29000000</t>
+          <t>33.50000000</t>
         </is>
       </c>
       <c r="I19" s="8" t="inlineStr">
@@ -1336,7 +1336,7 @@
       </c>
       <c r="B20" s="8" t="inlineStr">
         <is>
-          <t>3.29070000</t>
+          <t>3.32280000</t>
         </is>
       </c>
       <c r="C20" s="8" t="inlineStr">
@@ -1360,11 +1360,11 @@
         </is>
       </c>
       <c r="G20" s="8" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>3.16290000</t>
+          <t>3.19010000</t>
         </is>
       </c>
       <c r="I20" s="8" t="n"/>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B21" s="8" t="inlineStr">
         <is>
-          <t>19.84000000</t>
+          <t>20.99000000</t>
         </is>
       </c>
       <c r="C21" s="8" t="inlineStr">
@@ -1401,11 +1401,11 @@
         </is>
       </c>
       <c r="G21" s="8" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>19.17000000</t>
+          <t>19.04000000</t>
         </is>
       </c>
       <c r="I21" s="8" t="n"/>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="B22" s="8" t="inlineStr">
         <is>
-          <t>12.03400000</t>
+          <t>12.57900000</t>
         </is>
       </c>
       <c r="C22" s="8" t="inlineStr">
@@ -1442,11 +1442,11 @@
         </is>
       </c>
       <c r="G22" s="12" t="n">
-        <v>-22</v>
+        <v>-26</v>
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>10.68800000</t>
+          <t>11.21100000</t>
         </is>
       </c>
       <c r="I22" s="8" t="inlineStr">
@@ -1463,17 +1463,17 @@
       </c>
       <c r="B23" s="8" t="inlineStr">
         <is>
-          <t>0.17020000</t>
+          <t>0.17240000</t>
         </is>
       </c>
       <c r="C23" s="8" t="inlineStr">
         <is>
-          <t>0.15140000</t>
+          <t>0.15490000</t>
         </is>
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>13-12-21</t>
+          <t>14-12-21</t>
         </is>
       </c>
       <c r="E23" s="8" t="inlineStr">
@@ -1487,11 +1487,11 @@
         </is>
       </c>
       <c r="G23" s="8" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H23" s="8" t="inlineStr">
         <is>
-          <t>0.16510000</t>
+          <t>0.16610000</t>
         </is>
       </c>
       <c r="I23" s="8" t="n"/>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="B24" s="8" t="inlineStr">
         <is>
-          <t>5.28200000</t>
+          <t>6.17300000</t>
         </is>
       </c>
       <c r="C24" s="8" t="inlineStr">
@@ -1524,15 +1524,15 @@
       </c>
       <c r="F24" s="8" t="inlineStr">
         <is>
-          <t>6.07600000</t>
+          <t>6.29900000</t>
         </is>
       </c>
       <c r="G24" s="12" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H24" s="8" t="inlineStr">
         <is>
-          <t>4.65500000</t>
+          <t>5.00300000</t>
         </is>
       </c>
       <c r="I24" s="8" t="n"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B25" s="8" t="inlineStr">
         <is>
-          <t>8.36100000</t>
+          <t>8.36800000</t>
         </is>
       </c>
       <c r="C25" s="8" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>8.23100000</t>
+          <t>7.87700000</t>
         </is>
       </c>
       <c r="I25" s="8" t="n"/>
@@ -1586,17 +1586,17 @@
       </c>
       <c r="B26" s="8" t="inlineStr">
         <is>
-          <t>308.80000000</t>
+          <t>335.40000000</t>
         </is>
       </c>
       <c r="C26" s="8" t="inlineStr">
         <is>
-          <t>211.90000000</t>
+          <t>212.70000000</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>13-12-21</t>
+          <t>14-12-21</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
@@ -1610,11 +1610,11 @@
         </is>
       </c>
       <c r="G26" s="8" t="n">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>306.80000000</t>
+          <t>304.90000000</t>
         </is>
       </c>
       <c r="I26" s="8" t="n"/>
@@ -1627,17 +1627,17 @@
       </c>
       <c r="B27" s="8" t="inlineStr">
         <is>
-          <t>0.07669000</t>
+          <t>0.07682000</t>
         </is>
       </c>
       <c r="C27" s="8" t="inlineStr">
         <is>
-          <t>0.07488000</t>
+          <t>0.07354000</t>
         </is>
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>20-12-21</t>
+          <t>31-12-21</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
@@ -1647,18 +1647,22 @@
       </c>
       <c r="F27" s="8" t="inlineStr">
         <is>
-          <t>0.09235000</t>
-        </is>
-      </c>
-      <c r="G27" s="8" t="n">
-        <v>20</v>
+          <t>0.08887000</t>
+        </is>
+      </c>
+      <c r="G27" s="12" t="n">
+        <v>15</v>
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>0.07561000</t>
-        </is>
-      </c>
-      <c r="I27" s="8" t="n"/>
+          <t>0.07354000</t>
+        </is>
+      </c>
+      <c r="I27" s="8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="8" t="inlineStr">
@@ -1668,17 +1672,17 @@
       </c>
       <c r="B28" s="8" t="inlineStr">
         <is>
-          <t>0.07669000</t>
+          <t>0.07682000</t>
         </is>
       </c>
       <c r="C28" s="8" t="inlineStr">
         <is>
-          <t>0.07488000</t>
+          <t>0.07354000</t>
         </is>
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>20-12-21</t>
+          <t>31-12-21</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
@@ -1688,18 +1692,22 @@
       </c>
       <c r="F28" s="8" t="inlineStr">
         <is>
-          <t>0.09235000</t>
-        </is>
-      </c>
-      <c r="G28" s="8" t="n">
-        <v>20</v>
+          <t>0.08887000</t>
+        </is>
+      </c>
+      <c r="G28" s="12" t="n">
+        <v>15</v>
       </c>
       <c r="H28" s="8" t="inlineStr">
         <is>
-          <t>0.07561000</t>
-        </is>
-      </c>
-      <c r="I28" s="8" t="n"/>
+          <t>0.07354000</t>
+        </is>
+      </c>
+      <c r="I28" s="8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="8" t="inlineStr">
@@ -1709,7 +1717,7 @@
       </c>
       <c r="B29" s="8" t="inlineStr">
         <is>
-          <t>31.36000000</t>
+          <t>35.30000000</t>
         </is>
       </c>
       <c r="C29" s="8" t="inlineStr">
@@ -1729,7 +1737,7 @@
       </c>
       <c r="F29" s="8" t="inlineStr">
         <is>
-          <t>32.70000000</t>
+          <t>37.00000000</t>
         </is>
       </c>
       <c r="G29" s="12" t="n">
@@ -1737,7 +1745,7 @@
       </c>
       <c r="H29" s="8" t="inlineStr">
         <is>
-          <t>25.10000000</t>
+          <t>30.11000000</t>
         </is>
       </c>
       <c r="I29" s="8" t="n"/>
@@ -1750,7 +1758,7 @@
       </c>
       <c r="B30" s="8" t="inlineStr">
         <is>
-          <t>1.43830000</t>
+          <t>1.39100000</t>
         </is>
       </c>
       <c r="C30" s="8" t="inlineStr">
@@ -1774,11 +1782,11 @@
         </is>
       </c>
       <c r="G30" s="12" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H30" s="8" t="inlineStr">
         <is>
-          <t>1.41200000</t>
+          <t>1.33410000</t>
         </is>
       </c>
       <c r="I30" s="8" t="n"/>
@@ -1791,7 +1799,7 @@
       </c>
       <c r="B31" s="8" t="inlineStr">
         <is>
-          <t>24.70000000</t>
+          <t>27.41000000</t>
         </is>
       </c>
       <c r="C31" s="8" t="inlineStr">
@@ -1814,12 +1822,12 @@
           <t>29.90000000</t>
         </is>
       </c>
-      <c r="G31" s="8" t="n">
-        <v>21</v>
+      <c r="G31" s="12" t="n">
+        <v>9</v>
       </c>
       <c r="H31" s="8" t="inlineStr">
         <is>
-          <t>23.26000000</t>
+          <t>24.00000000</t>
         </is>
       </c>
       <c r="I31" s="8" t="n"/>
@@ -1832,7 +1840,7 @@
       </c>
       <c r="B32" s="8" t="inlineStr">
         <is>
-          <t>147.60000000</t>
+          <t>149.70000000</t>
         </is>
       </c>
       <c r="C32" s="8" t="inlineStr">
@@ -1856,11 +1864,11 @@
         </is>
       </c>
       <c r="G32" s="12" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>142.70000000</t>
+          <t>143.70000000</t>
         </is>
       </c>
       <c r="I32" s="8" t="n"/>
@@ -1873,7 +1881,7 @@
       </c>
       <c r="B33" s="8" t="inlineStr">
         <is>
-          <t>1.23300000</t>
+          <t>1.22400000</t>
         </is>
       </c>
       <c r="C33" s="8" t="inlineStr">
@@ -1897,11 +1905,11 @@
         </is>
       </c>
       <c r="G33" s="8" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H33" s="8" t="inlineStr">
         <is>
-          <t>1.22800000</t>
+          <t>1.18200000</t>
         </is>
       </c>
       <c r="I33" s="8" t="n"/>
@@ -1914,7 +1922,7 @@
       </c>
       <c r="B34" s="8" t="inlineStr">
         <is>
-          <t>0.08357000</t>
+          <t>0.08592000</t>
         </is>
       </c>
       <c r="C34" s="8" t="inlineStr">
@@ -1938,11 +1946,11 @@
         </is>
       </c>
       <c r="G34" s="8" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H34" s="8" t="inlineStr">
         <is>
-          <t>0.08065000</t>
+          <t>0.08086000</t>
         </is>
       </c>
       <c r="I34" s="8" t="n"/>
@@ -1955,17 +1963,17 @@
       </c>
       <c r="B35" s="8" t="inlineStr">
         <is>
-          <t>4.69200000</t>
+          <t>4.86800000</t>
         </is>
       </c>
       <c r="C35" s="8" t="inlineStr">
         <is>
-          <t>3.81200000</t>
+          <t>3.82500000</t>
         </is>
       </c>
       <c r="D35" s="8" t="inlineStr">
         <is>
-          <t>13-12-21</t>
+          <t>14-12-21</t>
         </is>
       </c>
       <c r="E35" s="8" t="inlineStr">
@@ -1979,11 +1987,11 @@
         </is>
       </c>
       <c r="G35" s="8" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H35" s="8" t="inlineStr">
         <is>
-          <t>4.67400000</t>
+          <t>4.56100000</t>
         </is>
       </c>
       <c r="I35" s="8" t="n"/>
@@ -1996,7 +2004,7 @@
       </c>
       <c r="B36" s="8" t="inlineStr">
         <is>
-          <t>17.83000000</t>
+          <t>17.36000000</t>
         </is>
       </c>
       <c r="C36" s="8" t="inlineStr">
@@ -2020,11 +2028,11 @@
         </is>
       </c>
       <c r="G36" s="12" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>16.71000000</t>
+          <t>16.77000000</t>
         </is>
       </c>
       <c r="I36" s="8" t="n"/>
@@ -2037,7 +2045,7 @@
       </c>
       <c r="B37" s="8" t="inlineStr">
         <is>
-          <t>0.40490000</t>
+          <t>0.42770000</t>
         </is>
       </c>
       <c r="C37" s="8" t="inlineStr">
@@ -2057,15 +2065,15 @@
       </c>
       <c r="F37" s="8" t="inlineStr">
         <is>
-          <t>0.42900000</t>
+          <t>0.45460000</t>
         </is>
       </c>
       <c r="G37" s="12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H37" s="8" t="inlineStr">
         <is>
-          <t>0.34045000</t>
+          <t>0.39142000</t>
         </is>
       </c>
       <c r="I37" s="8" t="n"/>
@@ -2078,17 +2086,17 @@
       </c>
       <c r="B38" s="8" t="inlineStr">
         <is>
-          <t>94.36000000</t>
+          <t>93.91000000</t>
         </is>
       </c>
       <c r="C38" s="8" t="inlineStr">
         <is>
-          <t>100.43000000</t>
+          <t>103.51000000</t>
         </is>
       </c>
       <c r="D38" s="8" t="inlineStr">
         <is>
-          <t>12-12-21</t>
+          <t>25-12-21</t>
         </is>
       </c>
       <c r="E38" s="8" t="inlineStr">
@@ -2106,7 +2114,7 @@
       </c>
       <c r="H38" s="8" t="inlineStr">
         <is>
-          <t>91.80000000</t>
+          <t>91.10000000</t>
         </is>
       </c>
       <c r="I38" s="8" t="n"/>
@@ -2119,7 +2127,7 @@
       </c>
       <c r="B39" s="8" t="inlineStr">
         <is>
-          <t>0.04384000</t>
+          <t>0.04693000</t>
         </is>
       </c>
       <c r="C39" s="8" t="inlineStr">
@@ -2143,11 +2151,11 @@
         </is>
       </c>
       <c r="G39" s="8" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>0.04367000</t>
+          <t>0.04198000</t>
         </is>
       </c>
       <c r="I39" s="8" t="n"/>
@@ -2167,7 +2175,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F8"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -2231,7 +2239,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>11.90900000</t>
+          <t>12.60200000</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2240,7 +2248,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>-21</v>
+        <v>-26</v>
       </c>
     </row>
     <row r="3">
@@ -2251,22 +2259,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3710.24000000</t>
+          <t>3756.04000000</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4173.63000000</t>
+          <t>4150.00000000</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>4173.63000000</t>
-        </is>
-      </c>
+          <t>4150.00000000</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2276,7 +2285,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>35.36000000</t>
+          <t>35.69000000</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2285,7 +2294,12 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>41.27000000</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -2296,16 +2310,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>140.10000000</t>
+          <t>189.80000000</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>97.70000000</t>
+          <t>96.80000000</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>-30</v>
+        <v>-48</v>
       </c>
     </row>
     <row r="6">
@@ -2316,7 +2330,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>46886.31000000</t>
+          <t>47421.71000000</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2325,7 +2339,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -2341,66 +2355,67 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>510.70000000</t>
+          <t>524.30000000</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>574.80000000</t>
+          <t>572.00000000</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>574.80000000</t>
-        </is>
-      </c>
+          <t>572.00000000</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>FTMUSDT</t>
+          <t>AVAXUSDT</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2.09460000</t>
+          <t>116.28000000</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2.44880000</t>
+          <t>87.46000000</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>16</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2.44880000</t>
-        </is>
+        <v>-24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>AVAXUSDT</t>
+          <t>TRXUSDT</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>100.87000000</t>
+          <t>0.07691000</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>89.92000000</t>
+          <t>0.08887000</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-10</v>
+        <v>15</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0.08887000</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>